<commit_message>
after main menu redesign
</commit_message>
<xml_diff>
--- a/akm_design_layout.xlsx
+++ b/akm_design_layout.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="77" yWindow="111" windowWidth="19097" windowHeight="7311" activeTab="2"/>
+    <workbookView xWindow="80" yWindow="110" windowWidth="19100" windowHeight="7310" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
   <si>
     <r>
       <rPr>
@@ -935,13 +935,22 @@
   </si>
   <si>
     <t>Полное описание назначения сопровождаемой системы</t>
+  </si>
+  <si>
+    <t>Заголовок информационной панели</t>
+  </si>
+  <si>
+    <t>Пример</t>
+  </si>
+  <si>
+    <t>Информационный портал отдела ДБО ФЛ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1060,15 +1069,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="8"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1109,7 +1109,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="33">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -1513,43 +1513,139 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1560,24 +1656,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1587,54 +1665,6 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1650,94 +1680,95 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2047,154 +2078,161 @@
       <selection activeCell="J3" sqref="J3:L5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="19" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="25"/>
-      <c r="L1" s="26"/>
-    </row>
-    <row r="2" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="16" t="s">
+      <c r="K1" s="11"/>
+      <c r="L1" s="12"/>
+    </row>
+    <row r="2" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="19" t="s">
+      <c r="B2" s="14"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="26"/>
-    </row>
-    <row r="3" spans="1:12" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="33" t="s">
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="12"/>
+    </row>
+    <row r="3" spans="1:12" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="19" t="s">
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="27" t="s">
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="27"/>
-      <c r="L3" s="28"/>
-    </row>
-    <row r="4" spans="1:12" ht="110.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="34"/>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="35" t="s">
+      <c r="K3" s="18"/>
+      <c r="L3" s="19"/>
+    </row>
+    <row r="4" spans="1:12" ht="110.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="25"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="37"/>
-      <c r="J4" s="29"/>
-      <c r="K4" s="29"/>
-      <c r="L4" s="30"/>
-    </row>
-    <row r="5" spans="1:12" ht="29.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="19" t="s">
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="21"/>
+    </row>
+    <row r="5" spans="1:12" ht="29.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="25"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="40"/>
-      <c r="J5" s="31"/>
-      <c r="K5" s="31"/>
-      <c r="L5" s="32"/>
-    </row>
-    <row r="6" spans="1:12" ht="33.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="16" t="s">
+      <c r="B5" s="11"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="23"/>
+    </row>
+    <row r="6" spans="1:12" ht="33.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="19" t="s">
+      <c r="B6" s="14"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="22" t="s">
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="K6" s="23"/>
-      <c r="L6" s="24"/>
-    </row>
-    <row r="7" spans="1:12" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="14" t="s">
+      <c r="K6" s="36"/>
+      <c r="L6" s="37"/>
+    </row>
+    <row r="7" spans="1:12" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="19" t="s">
+      <c r="B7" s="34"/>
+      <c r="C7" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="19" t="s">
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="L7" s="20"/>
-    </row>
-    <row r="9" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="13" t="s">
+      <c r="L7" s="17"/>
+    </row>
+    <row r="9" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="32"/>
+      <c r="L9" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A9:L9"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="K7:L7"/>
+    <mergeCell ref="C7:J7"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="D6:I6"/>
     <mergeCell ref="D2:L2"/>
     <mergeCell ref="J1:L1"/>
     <mergeCell ref="A2:C2"/>
@@ -2204,13 +2242,6 @@
     <mergeCell ref="A3:C4"/>
     <mergeCell ref="A5:C5"/>
     <mergeCell ref="D4:I5"/>
-    <mergeCell ref="A9:L9"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="C7:J7"/>
-    <mergeCell ref="J6:L6"/>
-    <mergeCell ref="D6:I6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="83" orientation="portrait" r:id="rId1"/>
@@ -2225,107 +2256,107 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="45" t="s">
+    <row r="1" spans="1:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="20"/>
-    </row>
-    <row r="2" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="42" t="s">
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="17"/>
+    </row>
+    <row r="2" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="44"/>
-    </row>
-    <row r="3" spans="1:12" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="19" t="s">
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="41"/>
+    </row>
+    <row r="3" spans="1:12" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="20"/>
-    </row>
-    <row r="4" spans="1:12" ht="110.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="19" t="s">
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="17"/>
+    </row>
+    <row r="4" spans="1:12" ht="110.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="33" t="s">
+      <c r="B4" s="16"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="29"/>
-      <c r="K4" s="29"/>
-      <c r="L4" s="30"/>
-    </row>
-    <row r="5" spans="1:12" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="19" t="s">
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="21"/>
+    </row>
+    <row r="5" spans="1:12" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21"/>
-      <c r="L5" s="20"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A7" s="41" t="s">
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="17"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="41"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="41"/>
-      <c r="H7" s="41"/>
-      <c r="I7" s="41"/>
-      <c r="J7" s="41"/>
-      <c r="K7" s="41"/>
-      <c r="L7" s="41"/>
-    </row>
-    <row r="8" spans="1:12" s="1" customFormat="1" ht="14.5" x14ac:dyDescent="0.35"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="38"/>
+      <c r="K7" s="38"/>
+      <c r="L7" s="38"/>
+    </row>
+    <row r="8" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="A7:L7"/>
@@ -2343,455 +2374,489 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L40"/>
+  <dimension ref="A1:L41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" zoomScale="145" zoomScaleNormal="145" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26:D26"/>
+      <selection activeCell="B26" sqref="B26:H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="4" width="9.23046875" style="54"/>
+    <col min="2" max="4" width="9.26953125" style="8"/>
+    <col min="6" max="8" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="45" t="s">
+    <row r="1" spans="1:12" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="20"/>
-    </row>
-    <row r="2" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="42" t="s">
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="17"/>
+    </row>
+    <row r="2" spans="1:12" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="44"/>
-    </row>
-    <row r="3" spans="1:12" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="19" t="s">
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="41"/>
+    </row>
+    <row r="3" spans="1:12" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="20"/>
-    </row>
-    <row r="4" spans="1:12" ht="110.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="19" t="s">
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="17"/>
+    </row>
+    <row r="4" spans="1:12" ht="110.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="33" t="s">
+      <c r="B4" s="16"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="29"/>
-      <c r="K4" s="29"/>
-      <c r="L4" s="30"/>
-    </row>
-    <row r="5" spans="1:12" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="19" t="s">
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="21"/>
+    </row>
+    <row r="5" spans="1:12" ht="34" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21"/>
-      <c r="L5" s="20"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="A7" s="41" t="s">
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="17"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="41"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="41"/>
-      <c r="H7" s="41"/>
-      <c r="I7" s="41"/>
-      <c r="J7" s="41"/>
-      <c r="K7" s="41"/>
-      <c r="L7" s="41"/>
-    </row>
-    <row r="8" spans="1:12" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B8" s="46"/>
-      <c r="C8" s="46"/>
-      <c r="D8" s="46"/>
-    </row>
-    <row r="9" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B9" s="56" t="s">
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="38"/>
+      <c r="K7" s="38"/>
+      <c r="L7" s="38"/>
+    </row>
+    <row r="8" spans="1:12" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="F8" s="67"/>
+      <c r="G8" s="67"/>
+      <c r="H8" s="67"/>
+    </row>
+    <row r="9" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="57"/>
-      <c r="D9" s="57"/>
-      <c r="E9" s="11" t="s">
+      <c r="C9" s="58"/>
+      <c r="D9" s="58"/>
+      <c r="E9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="58"/>
-      <c r="G9" s="59"/>
-      <c r="H9" s="60"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="B10" s="67" t="s">
+      <c r="F9" s="64" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" s="65"/>
+      <c r="H9" s="66"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B10" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="68"/>
-      <c r="D10" s="68"/>
-      <c r="E10" s="68"/>
-      <c r="F10" s="68"/>
-      <c r="G10" s="68"/>
-      <c r="H10" s="69"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="B11" s="49" t="s">
+      <c r="C10" s="46"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="46"/>
+      <c r="H10" s="47"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B11" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="50"/>
-      <c r="D11" s="50"/>
-      <c r="E11" s="9">
+      <c r="C11" s="44"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="3">
         <v>8</v>
       </c>
-      <c r="F11" s="73"/>
-      <c r="G11" s="74"/>
-      <c r="H11" s="75"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="B12" s="49" t="s">
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="68"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B12" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="50"/>
-      <c r="D12" s="50"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="73"/>
-      <c r="G12" s="74"/>
-      <c r="H12" s="75"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="B13" s="49"/>
-      <c r="C13" s="50"/>
-      <c r="D13" s="50"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="73"/>
-      <c r="G13" s="74"/>
-      <c r="H13" s="75"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="B14" s="49"/>
-      <c r="C14" s="50"/>
-      <c r="D14" s="50"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="73"/>
-      <c r="G14" s="74"/>
-      <c r="H14" s="75"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="B15" s="49"/>
-      <c r="C15" s="50"/>
-      <c r="D15" s="50"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="73"/>
-      <c r="G15" s="74"/>
-      <c r="H15" s="75"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.4">
-      <c r="B16" s="49"/>
-      <c r="C16" s="50"/>
-      <c r="D16" s="50"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="73"/>
-      <c r="G16" s="74"/>
-      <c r="H16" s="75"/>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B17" s="70"/>
-      <c r="C17" s="71"/>
-      <c r="D17" s="72"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="61"/>
-      <c r="G17" s="62"/>
-      <c r="H17" s="63"/>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B18" s="70"/>
-      <c r="C18" s="71"/>
-      <c r="D18" s="72"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="61"/>
-      <c r="G18" s="62"/>
-      <c r="H18" s="63"/>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B19" s="47"/>
-      <c r="C19" s="48"/>
-      <c r="D19" s="48"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="61"/>
-      <c r="G19" s="62"/>
-      <c r="H19" s="63"/>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B20" s="64" t="s">
+      <c r="C12" s="44"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="68"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B13" s="43"/>
+      <c r="C13" s="44"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="68"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B14" s="43"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="68"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B15" s="43"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="68"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B16" s="43"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="68"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B17" s="51"/>
+      <c r="C17" s="52"/>
+      <c r="D17" s="53"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="69"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B18" s="51"/>
+      <c r="C18" s="52"/>
+      <c r="D18" s="53"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="69"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B19" s="59"/>
+      <c r="C19" s="60"/>
+      <c r="D19" s="60"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="69"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B20" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="65"/>
-      <c r="D20" s="65"/>
-      <c r="E20" s="65"/>
-      <c r="F20" s="65"/>
-      <c r="G20" s="65"/>
-      <c r="H20" s="66"/>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B21" s="47" t="s">
+      <c r="C20" s="49"/>
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="49"/>
+      <c r="G20" s="49"/>
+      <c r="H20" s="50"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B21" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="48"/>
-      <c r="D21" s="48"/>
-      <c r="E21" s="12">
+      <c r="C21" s="60"/>
+      <c r="D21" s="60"/>
+      <c r="E21" s="6">
         <v>10</v>
       </c>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="4"/>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B22" s="47" t="s">
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="69"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B22" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="48"/>
-      <c r="D22" s="48"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="4"/>
-    </row>
-    <row r="23" spans="2:8" ht="21.9" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="47" t="s">
+      <c r="C22" s="60"/>
+      <c r="D22" s="60"/>
+      <c r="E22" s="6">
         <v>25</v>
       </c>
-      <c r="C23" s="48"/>
-      <c r="D23" s="48"/>
-      <c r="E23" s="12">
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="69"/>
+    </row>
+    <row r="23" spans="2:8" ht="21.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="59" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="60"/>
+      <c r="D23" s="60"/>
+      <c r="E23" s="6">
         <v>50</v>
       </c>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="4"/>
-    </row>
-    <row r="24" spans="2:8" ht="22.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B24" s="47" t="s">
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="69"/>
+    </row>
+    <row r="24" spans="2:8" ht="22.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="48"/>
-      <c r="D24" s="48"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="4"/>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B25" s="64" t="s">
+      <c r="C24" s="60"/>
+      <c r="D24" s="60"/>
+      <c r="E24" s="6">
+        <v>200</v>
+      </c>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="69"/>
+    </row>
+    <row r="25" spans="2:8" ht="22.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="61" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="62"/>
+      <c r="D25" s="63"/>
+      <c r="E25" s="3">
+        <v>40</v>
+      </c>
+      <c r="F25" s="70" t="s">
+        <v>38</v>
+      </c>
+      <c r="G25" s="71"/>
+      <c r="H25" s="72"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B26" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="C25" s="65"/>
-      <c r="D25" s="65"/>
-      <c r="E25" s="65"/>
-      <c r="F25" s="65"/>
-      <c r="G25" s="65"/>
-      <c r="H25" s="66"/>
-    </row>
-    <row r="26" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B26" s="49" t="s">
+      <c r="C26" s="49"/>
+      <c r="D26" s="49"/>
+      <c r="E26" s="49"/>
+      <c r="F26" s="49"/>
+      <c r="G26" s="49"/>
+      <c r="H26" s="50"/>
+    </row>
+    <row r="27" spans="2:8" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="50"/>
-      <c r="D26" s="50"/>
-      <c r="E26" s="9">
+      <c r="C27" s="44"/>
+      <c r="D27" s="44"/>
+      <c r="E27" s="3">
         <v>15</v>
       </c>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="6"/>
-    </row>
-    <row r="27" spans="2:8" ht="22.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B27" s="49" t="s">
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="68"/>
+    </row>
+    <row r="28" spans="2:8" ht="22.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="50"/>
-      <c r="D27" s="50"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="6"/>
-    </row>
-    <row r="28" spans="2:8" ht="22.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B28" s="49" t="s">
+      <c r="C28" s="44"/>
+      <c r="D28" s="44"/>
+      <c r="E28" s="3">
+        <v>50</v>
+      </c>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="68"/>
+    </row>
+    <row r="29" spans="2:8" ht="22.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="C28" s="50"/>
-      <c r="D28" s="50"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="6"/>
-    </row>
-    <row r="29" spans="2:8" ht="23.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B29" s="49" t="s">
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="3">
+        <v>50</v>
+      </c>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="68"/>
+    </row>
+    <row r="30" spans="2:8" ht="23.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="C29" s="50"/>
-      <c r="D29" s="50"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="6"/>
-    </row>
-    <row r="30" spans="2:8" ht="23.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B30" s="49"/>
-      <c r="C30" s="50"/>
-      <c r="D30" s="50"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="6"/>
-    </row>
-    <row r="31" spans="2:8" ht="23.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B31" s="49"/>
-      <c r="C31" s="50"/>
-      <c r="D31" s="50"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="6"/>
-    </row>
-    <row r="32" spans="2:8" ht="23.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B32" s="49"/>
-      <c r="C32" s="50"/>
-      <c r="D32" s="50"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="6"/>
-    </row>
-    <row r="33" spans="2:8" ht="23.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B33" s="49"/>
-      <c r="C33" s="50"/>
-      <c r="D33" s="50"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
-      <c r="H33" s="6"/>
-    </row>
-    <row r="34" spans="2:8" ht="23.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B34" s="49"/>
-      <c r="C34" s="50"/>
-      <c r="D34" s="50"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
-      <c r="H34" s="6"/>
-    </row>
-    <row r="35" spans="2:8" ht="23.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B35" s="49"/>
-      <c r="C35" s="50"/>
-      <c r="D35" s="50"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
-      <c r="H35" s="6"/>
-    </row>
-    <row r="36" spans="2:8" ht="23.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B36" s="49"/>
-      <c r="C36" s="50"/>
-      <c r="D36" s="50"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
-      <c r="H36" s="6"/>
-    </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B37" s="49"/>
-      <c r="C37" s="50"/>
-      <c r="D37" s="50"/>
-      <c r="E37" s="9"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
-      <c r="H37" s="6"/>
-    </row>
-    <row r="38" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B38" s="51"/>
-      <c r="C38" s="52"/>
-      <c r="D38" s="52"/>
-      <c r="E38" s="10"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="7"/>
-      <c r="H38" s="8"/>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B39" s="53"/>
-      <c r="C39" s="53"/>
-      <c r="D39" s="53"/>
-      <c r="E39" s="2"/>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="C40" s="55"/>
-      <c r="D40" s="55"/>
+      <c r="C30" s="44"/>
+      <c r="D30" s="44"/>
+      <c r="E30" s="3">
+        <v>200</v>
+      </c>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="68"/>
+    </row>
+    <row r="31" spans="2:8" ht="23.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B31" s="43"/>
+      <c r="C31" s="44"/>
+      <c r="D31" s="44"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="68"/>
+    </row>
+    <row r="32" spans="2:8" ht="23.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B32" s="43"/>
+      <c r="C32" s="44"/>
+      <c r="D32" s="44"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="68"/>
+    </row>
+    <row r="33" spans="2:8" ht="23.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B33" s="43"/>
+      <c r="C33" s="44"/>
+      <c r="D33" s="44"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="68"/>
+    </row>
+    <row r="34" spans="2:8" ht="23.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B34" s="43"/>
+      <c r="C34" s="44"/>
+      <c r="D34" s="44"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="68"/>
+    </row>
+    <row r="35" spans="2:8" ht="23.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B35" s="43"/>
+      <c r="C35" s="44"/>
+      <c r="D35" s="44"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="68"/>
+    </row>
+    <row r="36" spans="2:8" ht="23.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B36" s="43"/>
+      <c r="C36" s="44"/>
+      <c r="D36" s="44"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="68"/>
+    </row>
+    <row r="37" spans="2:8" ht="23.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B37" s="43"/>
+      <c r="C37" s="44"/>
+      <c r="D37" s="44"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="68"/>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B38" s="43"/>
+      <c r="C38" s="44"/>
+      <c r="D38" s="44"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="68"/>
+    </row>
+    <row r="39" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B39" s="54"/>
+      <c r="C39" s="55"/>
+      <c r="D39" s="55"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="73"/>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B40" s="56"/>
+      <c r="C40" s="56"/>
+      <c r="D40" s="56"/>
       <c r="E40" s="2"/>
     </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="38">
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B10:H10"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B36:D36"/>
+  <mergeCells count="41">
     <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="B25:H25"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="A7:L7"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B26:H26"/>
     <mergeCell ref="B20:H20"/>
     <mergeCell ref="B18:D18"/>
     <mergeCell ref="A5:L5"/>
@@ -2800,22 +2865,22 @@
     <mergeCell ref="A3:L3"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="D4:L4"/>
-    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="F25:H25"/>
     <mergeCell ref="B37:D37"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="A7:L7"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="B12:D12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="83" orientation="portrait" r:id="rId1"/>
@@ -2828,7 +2893,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2840,7 +2905,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>